<commit_message>
optimisation du code products.js
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moi\Desktop\OPENCLASSROOMS\P5-Dev-Web-Kanap\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="7140"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -34,35 +42,109 @@
     <t>Affichage de l'ensemble des produits</t>
   </si>
   <si>
-    <t>OK / Description erreur</t>
-  </si>
-  <si>
     <t>...</t>
+  </si>
+  <si>
+    <t>Une page “produit” qui affiche (de manière dynamique) les détails du produit sur lequel l'utilisateur a cliqué depuis la page d’accueil.</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page produit dans le même navigateur</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page panier dans le même navigateur</t>
+  </si>
+  <si>
+    <t>~ possibilité de modifier la quantité d’un produit sélectionné ou bien de supprimer celui-ci.
+~ Contrôle des champs du formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une page “panier”. Celle-ci contient plusieurs parties : 
+- Un résumé des produits dans le panier, le prix total,
+- Un formulaire permettant de passer une commande.
+</t>
+  </si>
+  <si>
+    <t>Une page “confirmation”  de l'achat effectué</t>
+  </si>
+  <si>
+    <t>Ouvri sur la page confirmation avec le numéro de commande</t>
+  </si>
+  <si>
+    <t>Un message de confirmation de commande, remerciant l'utilisateur pour sa commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fonctionne parfaitement, possibilité de modifier la quantité, de supprimer.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>La possibilité de modifier la couleur sans revenir dans la fiche produit aurais été un plus</t>
+    </r>
+  </si>
+  <si>
+    <t>Fonctionne mais l'information sur la quantité et la couleur est absente</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Affichage des information de l'article choisi</t>
+  </si>
+  <si>
+    <t>une liste déroulante affichant les differente couleur</t>
+  </si>
+  <si>
+    <t>Cliquer sur "sélectionner une couleur" sur la page produit</t>
+  </si>
+  <si>
+    <t>une liste déroulante contenat les couleur disponible apparaait</t>
+  </si>
+  <si>
+    <t>ajout au panier</t>
+  </si>
+  <si>
+    <t>Cliquer sur "ajouter au panier" en emttant une quantité ou une couleur incorrect</t>
+  </si>
+  <si>
+    <t>une erreur apparait lors du clique</t>
+  </si>
+  <si>
+    <t>Une erreur indiquant "" apparait pour prévenir l'utilisateur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="18.0"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Montserrat"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -71,7 +153,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -81,7 +163,13 @@
     </fill>
   </fills>
   <borders count="17">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="medium">
         <color rgb="FF000000"/>
@@ -95,8 +183,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -106,6 +196,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -120,6 +211,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -134,6 +226,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -142,17 +235,22 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -161,9 +259,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -172,9 +272,11 @@
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -189,8 +291,10 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -200,6 +304,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -214,6 +319,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -228,6 +334,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="medium">
@@ -242,8 +349,10 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -253,6 +362,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -267,6 +377,7 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -281,92 +392,99 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -556,26 +674,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="7.29"/>
-    <col customWidth="1" min="2" max="3" width="58.43"/>
-    <col customWidth="1" min="4" max="4" width="57.86"/>
-    <col customWidth="1" min="5" max="5" width="52.71"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
+    <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="57.85546875" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" customHeight="1">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -590,174 +714,261 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="36">
       <c r="A2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="54">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="11"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="11"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:5" ht="18">
+      <c r="A8" s="11"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:5" ht="18">
+      <c r="A9" s="11"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="10" spans="1:5" ht="90">
+      <c r="A10" s="7">
+        <v>3</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="72">
+      <c r="A11" s="7">
+        <v>4</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18">
+      <c r="A12" s="7">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" ht="18">
+      <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="9">
-        <v>2.0</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="17"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="17"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="17"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="18"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="18">
+      <c r="A14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:5" ht="18">
+      <c r="A15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:5" ht="18">
+      <c r="A16" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="18">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="18">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="18">
+      <c r="A19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:5" ht="18">
+      <c r="A20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="11"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="11"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="18">
+      <c r="A23" s="11"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="18">
+      <c r="A24" s="11"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="18">
+      <c r="A25" s="11"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:5" ht="18">
+      <c r="A26" s="11"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" ht="18">
+      <c r="A27" s="11"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" ht="18">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finalisation code pour soutenance
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Feuille 1'!$A$1:$E$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -46,9 +49,6 @@
   </si>
   <si>
     <t>Une page “produit” qui affiche (de manière dynamique) les détails du produit sur lequel l'utilisateur a cliqué depuis la page d’accueil.</t>
-  </si>
-  <si>
-    <t>Ouvrir sur la page produit dans le même navigateur</t>
   </si>
   <si>
     <t>Ouvrir sur la page panier dans le même navigateur</t>
@@ -73,38 +73,12 @@
     <t>Un message de confirmation de commande, remerciant l'utilisateur pour sa commande, et indiquant l'identifiant de commande envoyé par l’API.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Fonctionne parfaitement, possibilité de modifier la quantité, de supprimer.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>La possibilité de modifier la couleur sans revenir dans la fiche produit aurais été un plus</t>
-    </r>
-  </si>
-  <si>
-    <t>Fonctionne mais l'information sur la quantité et la couleur est absente</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>Affichage des information de l'article choisi</t>
-  </si>
-  <si>
-    <t>une liste déroulante affichant les differente couleur</t>
-  </si>
-  <si>
     <t>Cliquer sur "sélectionner une couleur" sur la page produit</t>
   </si>
   <si>
-    <t>une liste déroulante contenat les couleur disponible apparaait</t>
-  </si>
-  <si>
     <t>ajout au panier</t>
   </si>
   <si>
@@ -114,7 +88,100 @@
     <t>une erreur apparait lors du clique</t>
   </si>
   <si>
-    <t>Une erreur indiquant "" apparait pour prévenir l'utilisateur</t>
+    <t>un input de quantité</t>
+  </si>
+  <si>
+    <t>cliquer pour choisir une quantié</t>
+  </si>
+  <si>
+    <t>le nomber de produit voulu est incrémenté</t>
+  </si>
+  <si>
+    <t>une liste déroulante contenat les couleur disponible apparait</t>
+  </si>
+  <si>
+    <t>quantité inférieur a 0</t>
+  </si>
+  <si>
+    <t>chiffre en dessous du zéro</t>
+  </si>
+  <si>
+    <t>Une erreur indiquant à l'utilisateur de choisir une quantité entre 0 et 100</t>
+  </si>
+  <si>
+    <t>quantité supérieur à 100 dans le cart</t>
+  </si>
+  <si>
+    <t>chiffre au dessus de 100</t>
+  </si>
+  <si>
+    <t>Une erreur indiquant à l'utilisateur de choisir une quantité couleur et une quantité</t>
+  </si>
+  <si>
+    <t>Cliquer sur "ajouter au panier" en eayant choisi une couleur et une quantité</t>
+  </si>
+  <si>
+    <t>message invitant l'utilisateur à aller dans la page du caddie</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>cliquer pour modifier la quantié</t>
+  </si>
+  <si>
+    <t>le nombre de produit voulu est incrémenté</t>
+  </si>
+  <si>
+    <t>bouton pour supprimer produit</t>
+  </si>
+  <si>
+    <t>supprime le produit</t>
+  </si>
+  <si>
+    <t>message demandant confirmation de la suppression</t>
+  </si>
+  <si>
+    <t>un formulaire pour saisir : nom, prénom, adresse, ville et mail</t>
+  </si>
+  <si>
+    <t>message sous chaque champ si un caractere non autorisé est saisi et si inférieur à 2</t>
+  </si>
+  <si>
+    <t>un bouton "Commander"</t>
+  </si>
+  <si>
+    <t>les informations de l'utilisateur sont saisies</t>
+  </si>
+  <si>
+    <t>enregistre la liste d'achat et les informations utilisateurs saisie dans les champs</t>
+  </si>
+  <si>
+    <t>l'utilisateur est dirigé vers la page de confirmation d'achat</t>
+  </si>
+  <si>
+    <t>aucun produit dans le panier</t>
+  </si>
+  <si>
+    <t>message alertant que le panier est vide, l'utilisateur est dirigé vers la page produit</t>
+  </si>
+  <si>
+    <t>information formulaire non complète ou erronée</t>
+  </si>
+  <si>
+    <t>message alertant que le formulaire est mal saisie</t>
+  </si>
+  <si>
+    <t>l'utilisateur reste sur la page caddie pour saisir ses informations</t>
+  </si>
+  <si>
+    <t>Ouvrir sur la page produite dans le même navigateur</t>
+  </si>
+  <si>
+    <t>Affichage des informations de l'article choisi</t>
+  </si>
+  <si>
+    <t>une liste déroulante affichant les differentes couleurs</t>
   </si>
 </sst>
 </file>
@@ -140,12 +207,16 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Montserrat"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
     <font>
       <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Montserrat"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -412,27 +483,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -446,25 +511,31 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,11 +754,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -715,260 +787,434 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="36">
-      <c r="A2" s="5">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="54">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36">
+      <c r="A4" s="22">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="22">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="36">
+      <c r="A6" s="22">
+        <v>5</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="36">
+      <c r="A7" s="22">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="54">
+      <c r="A8" s="22">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="54">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="19" t="s">
+      <c r="D8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="36">
+      <c r="A9" s="22">
         <v>8</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="B9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="72">
+      <c r="A10" s="22">
+        <v>3</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="36">
-      <c r="A4" s="11">
-        <v>3</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="D10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18">
+      <c r="A11" s="22">
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="36">
-      <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="C11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="36">
+      <c r="A12" s="22">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E12" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18">
-      <c r="A6" s="11"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" ht="18">
-      <c r="A7" s="11"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" ht="18">
-      <c r="A8" s="11"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" ht="18">
-      <c r="A9" s="11"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" ht="90">
-      <c r="A10" s="7">
-        <v>3</v>
-      </c>
-      <c r="B10" s="19" t="s">
+    <row r="13" spans="1:5" ht="36">
+      <c r="A13" s="22">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="36">
+      <c r="A14" s="22">
         <v>12</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="21" t="s">
+      <c r="B14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="36">
+      <c r="A15" s="22">
+        <v>13</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="36">
+      <c r="A16" s="22">
+        <v>14</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="36">
+      <c r="A17" s="22">
+        <v>15</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="36">
+      <c r="A18" s="22">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="72">
-      <c r="A11" s="7">
-        <v>4</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="B18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72">
+      <c r="A19" s="22">
+        <v>17</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="D19" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18">
-      <c r="A12" s="7">
-        <v>5</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" spans="1:5" ht="18">
-      <c r="A13" s="7" t="s">
+      <c r="E19" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18">
+      <c r="A20" s="22"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" spans="1:5" ht="18">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:5" ht="18">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" ht="18">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="18">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="18">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" ht="18">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="18">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="18">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="18">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="18">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" ht="18">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" ht="18">
-      <c r="A26" s="11"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" ht="18">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="9"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="18">
+      <c r="A30" s="9"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" ht="18">
+      <c r="A31" s="9"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="18">
+      <c r="A32" s="9"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" ht="18">
+      <c r="A33" s="9"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" ht="18">
+      <c r="A34" s="9"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" ht="18">
+      <c r="A35" s="9"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="18">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>